<commit_message>
Export review comments as XLSX
</commit_message>
<xml_diff>
--- a/app/static/templates/reviewCommentsTemplate.xlsx
+++ b/app/static/templates/reviewCommentsTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="Codelists" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Result Displays" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Analysis Results" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="All Comments" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t xml:space="preserve">Review Comments Summary</t>
   </si>
@@ -40,24 +41,6 @@
     <t xml:space="preserve">Resolved comments</t>
   </si>
   <si>
-    <t xml:space="preserve">Standards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datasets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codelists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result Displays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analysis Results</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -67,19 +50,7 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Created At</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modified At</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved At</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replies</t>
+    <t xml:space="preserve">Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Dataset</t>
@@ -98,6 +69,33 @@
   </si>
   <si>
     <t xml:space="preserve">Analysis Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifiedAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resolvedAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resolvedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reviewCommentOids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sources</t>
   </si>
 </sst>
 </file>
@@ -418,16 +416,15 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.9540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,45 +445,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>8</v>
-      </c>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>9</v>
-      </c>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
     </row>
@@ -509,47 +494,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -568,47 +538,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -627,49 +581,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -688,43 +630,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -743,44 +673,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -799,48 +717,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="106.372448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -852,4 +757,70 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>